<commit_message>
Verbesserte Augmentation, Doku, Statistik-Feldstudie
</commit_message>
<xml_diff>
--- a/Statistik/TabellarischerÜberblick.xlsx
+++ b/Statistik/TabellarischerÜberblick.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\anni\Documents\GitHub\CoopDFKI\Statistik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F77E1346-2593-4D48-A704-74505827A608}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1080951C-257F-40C0-9EE9-C54954BB8CE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{2D17CF7A-5CE0-4F1B-AC59-09188A30594C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve">Trainingstestreihe </t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ergebnisse: </t>
+  </si>
+  <si>
+    <t>Durchschnitt der F1-Werte</t>
+  </si>
+  <si>
+    <t>Netz: InceptionV3</t>
   </si>
 </sst>
 </file>
@@ -169,7 +175,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -177,13 +183,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -498,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BA1C09-5ECE-4B3F-A3CF-0DFDEF5558CC}">
-  <dimension ref="A2:AD18"/>
+  <dimension ref="A2:AD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,166 +561,235 @@
       <c r="G2" t="s">
         <v>32</v>
       </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B11">
         <v>0.1</v>
       </c>
-      <c r="G10">
+      <c r="G11">
         <v>0.01</v>
       </c>
-      <c r="L10">
+      <c r="L11">
         <v>1E-3</v>
       </c>
-      <c r="Q10">
+      <c r="Q11">
         <v>0.1</v>
       </c>
-      <c r="V10">
+      <c r="V11">
         <v>0.01</v>
       </c>
-      <c r="AA10">
+      <c r="AA11">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="V12" t="s">
+      <c r="V13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W12" t="s">
+      <c r="W13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="X12" t="s">
+      <c r="X13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Y13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AA13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AB13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AC13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AD13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B14">
+        <f>AVERAGE(0.28, 0,   0,   0,   0,   0,   0.29, 0,   0,   0,   0,   0)</f>
+        <v>4.7500000000000007E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="B15">
+        <f>AVERAGE(0.15, 0,   0,   0.27, 0,   0,   0.32, 0,   0,   0,   0,   0)</f>
+        <v>6.1666666666666668E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="B16">
+        <f xml:space="preserve"> AVERAGE(0,   0,   0,   0.26, 0,   0.02, 0.2,  0,   0,   0.05, 0,   0)</f>
+        <v>4.4166666666666667E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="B17">
+        <f xml:space="preserve"> AVERAGE(0.36, 0,   0,   0.19, 0.05, 0.1,  0.32, 0,   0,   0.03, 0,   0)</f>
+        <v>8.7500000000000008E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="B18">
+        <f xml:space="preserve"> AVERAGE(0.21, 0.04, 0,   0.23, 0,   0,   0,   0,   0,   0.01, 0,   0.06)</f>
+        <v>4.5833333333333337E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>30</v>
+      </c>
+      <c r="B19">
+        <f xml:space="preserve"> AVERAGE( 0,   0,   0,   0.29, 0,   0.24, 0,   0,   0,   0.09, 0,   0)</f>
+        <v>5.1666666666666666E-2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B14:E19">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:AD20">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:AD19">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>